<commit_message>
Ajuste de recursos en escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/Escaleta_MA_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/Escaleta_MA_06_12_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado06\guion12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18495" windowHeight="7305"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$P$1:$P$173</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -274,12 +279,6 @@
     <t>En la imagen de la izquerda un poligono, sobre el plano, indicando las coordenadas de los vértices. La instrucción debe decir: Selecciona las coordenadas de la figura si se traslada cuatro unidades a la derecha (este es el ejemplo, se debe ajustar en cada caso). En las opciones de respuesta colocar lso tres, cuatro, cinco, etc, puntos que correspondan.</t>
   </si>
   <si>
-    <t>Determna los vértices iniciales</t>
-  </si>
-  <si>
-    <t>Actividad para identificar los vértices iniciales de una figura</t>
-  </si>
-  <si>
     <t>Se da una figura y se indica que corresponde a la imagen de la figura trasladada. Se pide indicar los vértices iniciales de la figura (es decir antes de realizar la traslación).</t>
   </si>
   <si>
@@ -461,9 +460,6 @@
     <t>Interactivo que analiza los ejes de simetría de diferentes polígono regulares.</t>
   </si>
   <si>
-    <t>Interactivo que explica los diferentes tipos de simetría.</t>
-  </si>
-  <si>
     <t>Identifica las imágenes que se generan por simetría de reflexión</t>
   </si>
   <si>
@@ -603,6 +599,15 @@
   </si>
   <si>
     <t>Competencias: noción de simetría, homotecia y teselado</t>
+  </si>
+  <si>
+    <t>Determna los vértices iniciales de una figura</t>
+  </si>
+  <si>
+    <t>Actividad para identificar los vértices iniciales de una figura trasladada</t>
+  </si>
+  <si>
+    <t>Interactivo que explica  los tipos de simetría</t>
   </si>
 </sst>
 </file>
@@ -1011,6 +1016,42 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1034,42 +1075,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,7 +1136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1166,7 +1171,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1378,8 +1383,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38:U38"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1394,10 +1399,10 @@
     <col min="8" max="8" width="11.7109375" style="20" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="20" customWidth="1"/>
     <col min="10" max="10" width="32.28515625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="20" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="20" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="20" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="20" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="20" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="20" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="32.28515625" style="21" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" style="20" customWidth="1"/>
     <col min="17" max="17" width="16.140625" style="20" customWidth="1"/>
@@ -1409,94 +1414,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="61" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="64" t="s">
-        <v>176</v>
-      </c>
-      <c r="G1" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="64" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="66" t="s">
+      <c r="I1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="P1" s="56" t="s">
+      <c r="N1" s="66"/>
+      <c r="O1" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="64" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="52"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="64"/>
     </row>
     <row r="3" spans="1:21" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1506,7 +1511,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>77</v>
@@ -1526,7 +1531,7 @@
         <v>64</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>33</v>
@@ -1535,22 +1540,22 @@
       <c r="N3" s="10"/>
       <c r="O3" s="19"/>
       <c r="P3" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q3" s="16">
         <v>5</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S3" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>48</v>
       </c>
       <c r="U3" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1558,16 +1563,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" t="s">
         <v>182</v>
       </c>
-      <c r="C4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" t="s">
-        <v>185</v>
-      </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="38" t="s">
@@ -1583,7 +1588,7 @@
         <v>49</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>26</v>
@@ -1598,19 +1603,19 @@
         <v>5</v>
       </c>
       <c r="R4" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="T4" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="S4" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="T4" s="40" t="s">
-        <v>185</v>
-      </c>
       <c r="U4" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1618,7 +1623,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>77</v>
@@ -1638,7 +1643,7 @@
         <v>66</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>26</v>
@@ -1647,22 +1652,22 @@
       <c r="N5" s="9"/>
       <c r="O5" s="28"/>
       <c r="P5" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="16">
         <v>5</v>
       </c>
       <c r="R5" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S5" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T5" s="41" t="s">
         <v>67</v>
       </c>
       <c r="U5" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1673,7 +1678,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>77</v>
@@ -1693,7 +1698,7 @@
         <v>68</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>26</v>
@@ -1708,19 +1713,19 @@
         <v>5</v>
       </c>
       <c r="R6" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S6" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T6" s="41" t="s">
         <v>69</v>
       </c>
       <c r="U6" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1728,7 +1733,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>77</v>
@@ -1748,7 +1753,7 @@
         <v>71</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>26</v>
@@ -1757,22 +1762,22 @@
       <c r="N7" s="9"/>
       <c r="O7" s="28"/>
       <c r="P7" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q7" s="16">
         <v>5</v>
       </c>
       <c r="R7" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S7" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T7" s="41" t="s">
         <v>70</v>
       </c>
       <c r="U7" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1783,7 +1788,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>77</v>
@@ -1803,7 +1808,7 @@
         <v>73</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>26</v>
@@ -1812,22 +1817,22 @@
       <c r="N8" s="9"/>
       <c r="O8" s="28"/>
       <c r="P8" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q8" s="16">
         <v>5</v>
       </c>
       <c r="R8" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S8" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T8" s="41" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="U8" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1838,7 +1843,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>77</v>
@@ -1858,7 +1863,7 @@
         <v>78</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>26</v>
@@ -1873,16 +1878,16 @@
         <v>5</v>
       </c>
       <c r="R9" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S9" s="46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="T9" s="41" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1893,10 +1898,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="27"/>
@@ -1913,18 +1918,18 @@
         <v>80</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="28"/>
       <c r="P10" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q10" s="34">
         <v>6</v>
@@ -1933,13 +1938,13 @@
         <v>28</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="T10" s="42" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="U10" s="29" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1950,10 +1955,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="27"/>
@@ -1970,7 +1975,7 @@
         <v>82</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>26</v>
@@ -2009,15 +2014,15 @@
         <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="27"/>
       <c r="G12" s="38" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="H12" s="27">
         <v>10</v>
@@ -2026,10 +2031,10 @@
         <v>25</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>85</v>
+        <v>192</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>26</v>
@@ -2039,7 +2044,7 @@
         <v>27</v>
       </c>
       <c r="O12" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>18</v>
@@ -2054,7 +2059,7 @@
         <v>29</v>
       </c>
       <c r="T12" s="42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="U12" s="29" t="s">
         <v>31</v>
@@ -2068,15 +2073,15 @@
         <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="27"/>
       <c r="G13" s="38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H13" s="27">
         <v>11</v>
@@ -2085,10 +2090,10 @@
         <v>25</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>26</v>
@@ -2098,10 +2103,10 @@
         <v>34</v>
       </c>
       <c r="O13" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q13" s="34">
         <v>6</v>
@@ -2113,7 +2118,7 @@
         <v>29</v>
       </c>
       <c r="T13" s="42" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="U13" s="29" t="s">
         <v>31</v>
@@ -2127,15 +2132,15 @@
         <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="27"/>
       <c r="G14" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H14" s="24">
         <v>12</v>
@@ -2144,10 +2149,10 @@
         <v>25</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>26</v>
@@ -2157,7 +2162,7 @@
         <v>37</v>
       </c>
       <c r="O14" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>18</v>
@@ -2172,7 +2177,7 @@
         <v>29</v>
       </c>
       <c r="T14" s="42" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U14" s="29" t="s">
         <v>31</v>
@@ -2186,17 +2191,17 @@
         <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2205,10 +2210,10 @@
         <v>25</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>26</v>
@@ -2218,7 +2223,7 @@
         <v>36</v>
       </c>
       <c r="O15" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>18</v>
@@ -2233,7 +2238,7 @@
         <v>29</v>
       </c>
       <c r="T15" s="42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="U15" s="29" t="s">
         <v>31</v>
@@ -2247,15 +2252,15 @@
         <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="27"/>
       <c r="G16" s="38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2264,20 +2269,20 @@
         <v>18</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N16" s="9"/>
       <c r="O16" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>18</v>
@@ -2289,13 +2294,13 @@
         <v>28</v>
       </c>
       <c r="S16" s="47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="T16" s="42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="U16" s="29" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -2306,15 +2311,15 @@
         <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="27"/>
       <c r="G17" s="38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H17" s="24">
         <v>15</v>
@@ -2323,10 +2328,10 @@
         <v>18</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>33</v>
@@ -2336,7 +2341,7 @@
       </c>
       <c r="N17" s="9"/>
       <c r="O17" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>18</v>
@@ -2365,15 +2370,15 @@
         <v>47</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="27"/>
       <c r="G18" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2382,10 +2387,10 @@
         <v>25</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>26</v>
@@ -2395,10 +2400,10 @@
         <v>32</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P18" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q18" s="34">
         <v>6</v>
@@ -2410,7 +2415,7 @@
         <v>29</v>
       </c>
       <c r="T18" s="42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U18" s="29" t="s">
         <v>31</v>
@@ -2424,10 +2429,10 @@
         <v>47</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="27"/>
@@ -2441,10 +2446,10 @@
         <v>25</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>26</v>
@@ -2454,7 +2459,7 @@
         <v>40</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>18</v>
@@ -2483,15 +2488,15 @@
         <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="27"/>
       <c r="G20" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H20" s="27">
         <v>18</v>
@@ -2503,7 +2508,7 @@
         <v>51</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>26</v>
@@ -2516,7 +2521,7 @@
         <v>52</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q20" s="34">
         <v>6</v>
@@ -2542,15 +2547,15 @@
         <v>47</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="27"/>
       <c r="G21" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H21" s="24">
         <v>19</v>
@@ -2559,10 +2564,10 @@
         <v>25</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>26</v>
@@ -2572,10 +2577,10 @@
         <v>27</v>
       </c>
       <c r="O21" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q21" s="34">
         <v>6</v>
@@ -2587,7 +2592,7 @@
         <v>29</v>
       </c>
       <c r="T21" s="42" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="U21" s="29" t="s">
         <v>31</v>
@@ -2601,10 +2606,10 @@
         <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>35</v>
@@ -2620,10 +2625,10 @@
         <v>25</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>26</v>
@@ -2633,7 +2638,7 @@
         <v>36</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>18</v>
@@ -2648,7 +2653,7 @@
         <v>29</v>
       </c>
       <c r="T22" s="42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="U22" s="29" t="s">
         <v>31</v>
@@ -2662,15 +2667,15 @@
         <v>47</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="31"/>
       <c r="G23" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -2679,10 +2684,10 @@
         <v>18</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>33</v>
@@ -2692,7 +2697,7 @@
       </c>
       <c r="N23" s="9"/>
       <c r="O23" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>18</v>
@@ -2721,15 +2726,15 @@
         <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="31"/>
       <c r="G24" s="38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H24" s="24">
         <v>22</v>
@@ -2738,10 +2743,10 @@
         <v>25</v>
       </c>
       <c r="J24" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>26</v>
@@ -2751,10 +2756,10 @@
         <v>45</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P24" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q24" s="34">
         <v>6</v>
@@ -2766,7 +2771,7 @@
         <v>29</v>
       </c>
       <c r="T24" s="42" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="U24" s="29" t="s">
         <v>31</v>
@@ -2780,15 +2785,15 @@
         <v>47</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="31"/>
       <c r="G25" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H25" s="27">
         <v>23</v>
@@ -2797,10 +2802,10 @@
         <v>25</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>26</v>
@@ -2810,7 +2815,7 @@
         <v>27</v>
       </c>
       <c r="O25" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P25" s="11" t="s">
         <v>18</v>
@@ -2825,7 +2830,7 @@
         <v>29</v>
       </c>
       <c r="T25" s="42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U25" s="29" t="s">
         <v>31</v>
@@ -2839,15 +2844,15 @@
         <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="31"/>
       <c r="G26" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -2856,10 +2861,10 @@
         <v>25</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>26</v>
@@ -2869,7 +2874,7 @@
         <v>27</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P26" s="11" t="s">
         <v>18</v>
@@ -2884,7 +2889,7 @@
         <v>29</v>
       </c>
       <c r="T26" s="42" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="U26" s="29" t="s">
         <v>31</v>
@@ -2898,17 +2903,17 @@
         <v>47</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>35</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -2917,10 +2922,10 @@
         <v>25</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>26</v>
@@ -2930,7 +2935,7 @@
         <v>36</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="P27" s="11" t="s">
         <v>18</v>
@@ -2945,7 +2950,7 @@
         <v>29</v>
       </c>
       <c r="T27" s="42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="U27" s="29" t="s">
         <v>31</v>
@@ -2959,10 +2964,10 @@
         <v>47</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="27"/>
@@ -2979,7 +2984,7 @@
         <v>58</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>19</v>
@@ -2996,16 +3001,16 @@
         <v>5</v>
       </c>
       <c r="R28" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S28" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T28" s="43" t="s">
         <v>59</v>
       </c>
       <c r="U28" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -3016,10 +3021,10 @@
         <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="27"/>
@@ -3033,10 +3038,10 @@
         <v>18</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>33</v>
@@ -3054,16 +3059,16 @@
         <v>5</v>
       </c>
       <c r="R29" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S29" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T29" s="43" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="U29" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -3074,15 +3079,15 @@
         <v>47</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="27"/>
       <c r="G30" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3091,10 +3096,10 @@
         <v>25</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L30" s="7" t="s">
         <v>26</v>
@@ -3102,7 +3107,7 @@
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>18</v>
@@ -3111,20 +3116,20 @@
         <v>5</v>
       </c>
       <c r="R30" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S30" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T30" s="43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U30" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="V30" s="50"/>
     </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
@@ -3132,15 +3137,15 @@
         <v>47</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="27"/>
       <c r="G31" s="38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H31" s="24">
         <v>29</v>
@@ -3152,7 +3157,7 @@
         <v>62</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L31" s="7" t="s">
         <v>26</v>
@@ -3160,25 +3165,25 @@
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P31" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q31" s="16">
         <v>5</v>
       </c>
       <c r="R31" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S31" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T31" s="43" t="s">
         <v>61</v>
       </c>
       <c r="U31" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -3189,10 +3194,10 @@
         <v>47</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="27"/>
@@ -3206,10 +3211,10 @@
         <v>18</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L32" s="7" t="s">
         <v>33</v>
@@ -3224,16 +3229,16 @@
         <v>5</v>
       </c>
       <c r="R32" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S32" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T32" s="43" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="U32" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3244,10 +3249,10 @@
         <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="27"/>
@@ -3264,7 +3269,7 @@
         <v>56</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L33" s="7" t="s">
         <v>26</v>
@@ -3279,16 +3284,16 @@
         <v>5</v>
       </c>
       <c r="R33" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S33" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T33" s="43" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="U33" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3299,15 +3304,15 @@
         <v>47</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="27"/>
       <c r="G34" s="38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3316,10 +3321,10 @@
         <v>25</v>
       </c>
       <c r="J34" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="K34" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>26</v>
@@ -3334,19 +3339,19 @@
         <v>5</v>
       </c>
       <c r="R34" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S34" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T34" s="43" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="U34" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>17</v>
       </c>
@@ -3354,15 +3359,15 @@
         <v>47</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="27"/>
       <c r="G35" s="38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H35" s="24">
         <v>33</v>
@@ -3371,10 +3376,10 @@
         <v>18</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L35" s="7" t="s">
         <v>19</v>
@@ -3383,25 +3388,25 @@
       <c r="N35" s="9"/>
       <c r="O35" s="19"/>
       <c r="P35" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q35" s="16">
         <v>5</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S35" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T35" s="43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U35" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>17</v>
       </c>
@@ -3409,15 +3414,15 @@
         <v>47</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="27"/>
       <c r="G36" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H36" s="27">
         <v>34</v>
@@ -3426,10 +3431,10 @@
         <v>25</v>
       </c>
       <c r="J36" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L36" s="7" t="s">
         <v>26</v>
@@ -3438,22 +3443,22 @@
       <c r="N36" s="9"/>
       <c r="O36" s="19"/>
       <c r="P36" s="11" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="Q36" s="16">
         <v>5</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S36" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T36" s="43" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="U36" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3464,15 +3469,15 @@
         <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="27"/>
       <c r="G37" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H37" s="27">
         <v>35</v>
@@ -3481,10 +3486,10 @@
         <v>25</v>
       </c>
       <c r="J37" s="30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L37" s="7" t="s">
         <v>26</v>
@@ -3495,20 +3500,20 @@
       <c r="P37" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Q37" s="70">
+      <c r="Q37" s="51">
         <v>5</v>
       </c>
       <c r="R37" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S37" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T37" s="43" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3519,13 +3524,13 @@
         <v>47</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="13"/>
       <c r="F38" s="27"/>
       <c r="G38" s="38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H38" s="24">
         <v>36</v>
@@ -3534,10 +3539,10 @@
         <v>25</v>
       </c>
       <c r="J38" s="30" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L38" s="7" t="s">
         <v>26</v>
@@ -3545,7 +3550,7 @@
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P38" s="11" t="s">
         <v>18</v>
@@ -3554,16 +3559,16 @@
         <v>5</v>
       </c>
       <c r="R38" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S38" s="48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="T38" s="41" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="U38" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -3574,13 +3579,13 @@
         <v>47</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="13"/>
       <c r="F39" s="27"/>
       <c r="G39" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H39" s="27">
         <v>37</v>
@@ -3589,10 +3594,10 @@
         <v>25</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L39" s="7" t="s">
         <v>43</v>
@@ -3617,13 +3622,13 @@
         <v>47</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="13"/>
       <c r="F40" s="27"/>
       <c r="G40" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H40" s="27">
         <v>38</v>
@@ -3632,10 +3637,10 @@
         <v>25</v>
       </c>
       <c r="J40" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L40" s="7" t="s">
         <v>26</v>
@@ -3660,7 +3665,7 @@
         <v>29</v>
       </c>
       <c r="T40" s="42" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="U40" s="29" t="s">
         <v>31</v>
@@ -3674,13 +3679,13 @@
         <v>47</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="13"/>
       <c r="F41" s="27"/>
       <c r="G41" s="38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H41" s="27">
         <v>39</v>
@@ -3689,10 +3694,10 @@
         <v>25</v>
       </c>
       <c r="J41" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="K41" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="L41" s="7" t="s">
         <v>26</v>
@@ -3702,7 +3707,7 @@
         <v>46</v>
       </c>
       <c r="O41" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P41" s="11" t="s">
         <v>18</v>
@@ -3717,7 +3722,7 @@
         <v>29</v>
       </c>
       <c r="T41" s="42" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="U41" s="29" t="s">
         <v>31</v>
@@ -5894,6 +5899,14 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -5906,14 +5919,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A41">

</xml_diff>